<commit_message>
Creating Training and Testing Datasets
</commit_message>
<xml_diff>
--- a/HT-timeline.xlsx
+++ b/HT-timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/odalysbar/Documents/HonorsThesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/odalysbar/Documents/HonorsThesis/HonorsThesis-TikTok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711738F4-8AB0-2A49-BD93-4124AEFD8DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B629292-064C-EE45-AAB5-6E95BD2FE48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="15140" windowHeight="13900" xr2:uid="{53C01A89-3AD8-5243-A432-31FD7721305A}"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="20880" windowHeight="14100" xr2:uid="{53C01A89-3AD8-5243-A432-31FD7721305A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,7 +467,7 @@
   <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>